<commit_message>
Ajustement même fichier que précédent
</commit_message>
<xml_diff>
--- a/Annexes/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/Annexes/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Robin/Desktop/Projet04/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967C2A97-AF07-8B42-BD51-BE0F82CA05BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30782332-8274-ED45-B87D-8D4A7FEE62E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="24660" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>